<commit_message>
ao: sch/sth may 2021 - apply recommendation from parteners
</commit_message>
<xml_diff>
--- a/SCH-STH/Baseline Mapping/Angola/May 2021/ao_sch_sth_baseline_1_school_wash_202105.xlsx
+++ b/SCH-STH/Baseline Mapping/Angola/May 2021/ao_sch_sth_baseline_1_school_wash_202105.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA148D1-26A7-426A-B1B7-E96710974FAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AED2B00-3FD3-4A47-885E-4F75DB324EB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4929" uniqueCount="1206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4932" uniqueCount="1209">
   <si>
     <t>type</t>
   </si>
@@ -3636,10 +3636,28 @@
     <t>Quantas turmas</t>
   </si>
   <si>
-    <t>selected(${w_consent}, '1.Sim') and selected(${w_toilet_available}, '1.Sim') and (not selected(${w_toilet_observation},'11.Could not observe'))</t>
-  </si>
-  <si>
-    <t>selected(${w_consent}, '1.Sim') and selected(${w_toilet_available}, '1.Sim') and  (not selected(${w_toilet_observation},'11.Could not observe'))</t>
+    <t>selected(${w_consent}, '1.Sim') and selected(${w_toilet_available}, '1.Sim') and (${w_toilet_observation} = '1.A.sanita.esta.limpa.(sem.urina,.fezes,.moscas)' or
+${w_toilet_observation} = '2.Agua.ou.outros.materiais.de.limpeza.pessoais.sao.evidentes' or
+${w_toilet_observation} = '3.Existe.uma.tampa.de.buraco' or
+${w_toilet_observation} = '4.Urina.na.pia' or
+${w_toilet_observation} = '5.Fezes.na.pia' or
+${w_toilet_observation} = '6.Urina.no.chao./.paredes' or
+${w_toilet_observation} = '7.Fezes.no.chao/paredes' or
+${w_toilet_observation} = '8.Odor' or
+${w_toilet_observation} = '9.Moscas.presentes' or
+${w_toilet_observation} = '10.Outros')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${w_consent}, '1.Sim') and selected(${w_toilet_available}, '1.Sim') </t>
+  </si>
+  <si>
+    <t>if(selected(.,'11.Nao.podia.observar'), count-selected(.)=1, true())</t>
+  </si>
+  <si>
+    <t>If "11.Could not observe" is selected, no other response is allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se "(11) Não podia observar" for selecionado, nenhuma outra resposta será permitida. </t>
   </si>
 </sst>
 </file>
@@ -3750,7 +3768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3782,6 +3800,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4065,10 +4084,10 @@
   <dimension ref="A1:P151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K61" sqref="K61"/>
+      <selection pane="bottomRight" activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5646,6 +5665,15 @@
       <c r="E103" t="s">
         <v>424</v>
       </c>
+      <c r="H103" t="s">
+        <v>1206</v>
+      </c>
+      <c r="I103" t="s">
+        <v>1207</v>
+      </c>
+      <c r="J103" t="s">
+        <v>1208</v>
+      </c>
       <c r="K103" t="s">
         <v>1139</v>
       </c>
@@ -5689,7 +5717,7 @@
       <c r="E106" t="s">
         <v>436</v>
       </c>
-      <c r="K106" t="s">
+      <c r="K106" s="15" t="s">
         <v>1204</v>
       </c>
       <c r="M106" t="s">
@@ -5951,8 +5979,8 @@
   <dimension ref="A1:I1064"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>